<commit_message>
Updates for latest blog post
</commit_message>
<xml_diff>
--- a/results/consolidated/2_user_per_second_stepup.xlsx
+++ b/results/consolidated/2_user_per_second_stepup.xlsx
@@ -1,20 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wip\serverlessJsScalingComparison\results\consolidated\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesrandall/Code/serverlessJsScalingComparison/results/consolidated/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73390C7-2AAA-2349-B863-D8B377AF2530}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1120" windowWidth="30880" windowHeight="19140" tabRatio="500"/>
+    <workbookView xWindow="1320" yWindow="1120" windowWidth="30880" windowHeight="19140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
     <sheet name="Throughput" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Performance!$A$3:$A$22</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Performance!$B$2</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Performance!$F$3:$F$22</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Performance!$B$3:$B$22</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Performance!$C$2</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Performance!$C$3:$C$22</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Performance!$D$2</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Performance!$D$3:$D$22</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Performance!$E$2</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Performance!$E$3:$E$22</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Performance!$F$2</definedName>
+  </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -28,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Time</t>
   </si>
@@ -48,9 +62,6 @@
     <t>Requests per Second</t>
   </si>
   <si>
-    <t>Azure Functions (Dec 17)</t>
-  </si>
-  <si>
     <t>Azure Functions (Mar 18)</t>
   </si>
   <si>
@@ -60,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -732,7 +743,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>Azure Functions (Dec 17)</c:v>
+                        <c:v>Azure Functions (Jan 18)</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1485,7 +1496,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Azure Functions - January</a:t>
+              <a:t>Azure Functions - Performance - January</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -1539,7 +1550,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Azure Functions (Dec 17)</c:v>
+                  <c:v>Azure Functions (Jan 18)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1880,6 +1891,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1363450800"/>
         <c:axId val="1363453120"/>
@@ -1887,21 +1899,21 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
               <c15:ser>
-                <c:idx val="0"/>
+                <c:idx val="1"/>
                 <c:order val="0"/>
                 <c:tx>
                   <c:strRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Performance!$B$2</c15:sqref>
+                          <c15:sqref>Performance!$C$2</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>User Load</c:v>
+                        <c:v>AWS Lambda</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1909,7 +1921,7 @@
                 <c:spPr>
                   <a:ln w="28575" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent1"/>
+                      <a:schemeClr val="accent2"/>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
@@ -1998,197 +2010,6 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Performance!$B$3:$B$22</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>0</c:formatCode>
-                      <c:ptCount val="20"/>
-                      <c:pt idx="0">
-                        <c:v>29</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>59</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>89</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>119</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>149</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>179</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>209</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>239</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>269</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>299</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>329</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>359</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>389</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>419</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>449</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>479</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>500</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>500</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>500</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>500</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000003-310B-407E-8542-3A4DBCA31BAB}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Performance!$C$2</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>AWS Lambda</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent2"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="none"/>
-                </c:marker>
-                <c:cat>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Performance!$A$3:$A$22</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>h:mm:ss</c:formatCode>
-                      <c:ptCount val="20"/>
-                      <c:pt idx="0">
-                        <c:v>1.7361111111111112E-4</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>3.4722222222222224E-4</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>5.2083333333333333E-4</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>6.9444444444444447E-4</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>8.6805555555555562E-4</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>1.0416666666666667E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>1.2152777777777778E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>1.3888888888888889E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>1.5625000000000001E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>1.7361111111111112E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>1.9097222222222224E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>2.0833333333333333E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>2.2569444444444442E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>2.4305555555555552E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>2.6041666666666661E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>2.777777777777777E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>2.9513888888888879E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>3.1249999999999989E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>3.2986111111111098E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>3.4722222222222207E-3</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:cat>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
                           <c15:sqref>Performance!$C$3:$C$22</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
@@ -2273,7 +2094,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Performance!$E$2</c15:sqref>
@@ -2302,7 +2123,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Performance!$A$3:$A$22</c15:sqref>
@@ -2377,7 +2198,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Performance!$E$3:$E$22</c15:sqref>
@@ -2451,7 +2272,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-310B-407E-8542-3A4DBCA31BAB}"/>
                   </c:ext>
@@ -2460,6 +2281,196 @@
             </c15:filteredLineSeries>
           </c:ext>
         </c:extLst>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>User Load</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Performance!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm:ss</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.7361111111111112E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4722222222222224E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.2083333333333333E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.9444444444444447E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.6805555555555562E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0416666666666667E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2152777777777778E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3888888888888889E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5625000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7361111111111112E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9097222222222224E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0833333333333333E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.2569444444444442E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.4305555555555552E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.6041666666666661E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.777777777777777E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.9513888888888879E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.1249999999999989E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.2986111111111098E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.4722222222222207E-3</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Performance!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>269</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>299</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>329</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>359</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>389</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>449</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>479</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-310B-407E-8542-3A4DBCA31BAB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="609083599"/>
+        <c:axId val="482177855"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="1363450800"/>
@@ -2623,6 +2634,65 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="482177855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="609083599"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="609083599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="h:mm:ss" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="482177855"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4070,7 +4140,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Throughput - January 18 vs March 18</a:t>
+              <a:t>Azure Functions - Throughput - January 18 vs March 18</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4472,7 +4542,7 @@
             <c15:filteredLineSeries>
               <c15:ser>
                 <c:idx val="1"/>
-                <c:order val="1"/>
+                <c:order val="0"/>
                 <c:tx>
                   <c:strRef>
                     <c:extLst>
@@ -4666,7 +4736,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Throughput!$E$2</c15:sqref>
@@ -4695,7 +4765,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Throughput!$A$3:$A$22</c15:sqref>
@@ -4770,7 +4840,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Throughput!$E$3:$E$22</c15:sqref>
@@ -4844,7 +4914,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-6C22-4B8B-9094-37E369BFB8FA}"/>
                   </c:ext>
@@ -4857,6 +4927,180 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Throughput!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>User Load</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Throughput!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm:ss</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.7361111111111112E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4722222222222224E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.2083333333333333E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.9444444444444447E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.6805555555555562E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0416666666666667E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2152777777777778E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3888888888888889E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5625000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7361111111111112E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9097222222222224E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0833333333333333E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.2569444444444442E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.4305555555555552E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.6041666666666661E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.777777777777777E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.9513888888888879E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.1249999999999989E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.2986111111111098E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.4722222222222207E-3</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Throughput!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>269</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>299</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>329</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>359</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>389</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>449</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>479</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6C22-4B8B-9094-37E369BFB8FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -4869,201 +5113,7 @@
         <c:smooth val="0"/>
         <c:axId val="1363506032"/>
         <c:axId val="1363502640"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Throughput!$B$2</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>User Load</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="none"/>
-                </c:marker>
-                <c:cat>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Throughput!$A$3:$A$22</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>h:mm:ss</c:formatCode>
-                      <c:ptCount val="20"/>
-                      <c:pt idx="0">
-                        <c:v>1.7361111111111112E-4</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>3.4722222222222224E-4</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>5.2083333333333333E-4</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>6.9444444444444447E-4</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>8.6805555555555562E-4</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>1.0416666666666667E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>1.2152777777777778E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>1.3888888888888889E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>1.5625000000000001E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>1.7361111111111112E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>1.9097222222222224E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>2.0833333333333333E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>2.2569444444444442E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>2.4305555555555552E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>2.6041666666666661E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>2.777777777777777E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>2.9513888888888879E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>3.1249999999999989E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>3.2986111111111098E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>3.4722222222222207E-3</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:cat>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Throughput!$B$3:$B$22</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>0</c:formatCode>
-                      <c:ptCount val="20"/>
-                      <c:pt idx="0">
-                        <c:v>29</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>59</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>89</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>119</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>149</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>179</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>209</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>239</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>269</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>299</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>329</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>359</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>389</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>419</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>449</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>479</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>500</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>500</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>500</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>500</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000003-6C22-4B8B-9094-37E369BFB8FA}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-          </c:ext>
-        </c:extLst>
+        <c:extLst/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="1363496928"/>
@@ -8064,28 +8114,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -8096,16 +8146,16 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1.7361111111111112E-4</v>
       </c>
@@ -8125,7 +8175,7 @@
         <v>0.33100000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A9" si="0">TIME(0,0,15)+A3</f>
         <v>3.4722222222222224E-4</v>
@@ -8146,7 +8196,7 @@
         <v>0.19500000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>5.2083333333333333E-4</v>
@@ -8167,7 +8217,7 @@
         <v>0.17100000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>6.9444444444444447E-4</v>
@@ -8188,7 +8238,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>8.6805555555555562E-4</v>
@@ -8209,7 +8259,7 @@
         <v>0.17499999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>1.0416666666666667E-3</v>
@@ -8230,7 +8280,7 @@
         <v>0.17299999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>1.2152777777777778E-3</v>
@@ -8251,7 +8301,7 @@
         <v>0.18099999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f t="shared" ref="A10:A20" si="1">TIME(0,0,15)+A9</f>
         <v>1.3888888888888889E-3</v>
@@ -8272,7 +8322,7 @@
         <v>0.193</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <f t="shared" si="1"/>
         <v>1.5625000000000001E-3</v>
@@ -8293,7 +8343,7 @@
         <v>0.193</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <f t="shared" si="1"/>
         <v>1.7361111111111112E-3</v>
@@ -8314,7 +8364,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f t="shared" si="1"/>
         <v>1.9097222222222224E-3</v>
@@ -8335,7 +8385,7 @@
         <v>0.223</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <f t="shared" si="1"/>
         <v>2.0833333333333333E-3</v>
@@ -8356,7 +8406,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <f t="shared" si="1"/>
         <v>2.2569444444444442E-3</v>
@@ -8377,7 +8427,7 @@
         <v>0.22600000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <f t="shared" si="1"/>
         <v>2.4305555555555552E-3</v>
@@ -8398,7 +8448,7 @@
         <v>0.24099999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <f t="shared" si="1"/>
         <v>2.6041666666666661E-3</v>
@@ -8419,7 +8469,7 @@
         <v>0.23699999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <f t="shared" si="1"/>
         <v>2.777777777777777E-3</v>
@@ -8440,7 +8490,7 @@
         <v>0.23200000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <f t="shared" si="1"/>
         <v>2.9513888888888879E-3</v>
@@ -8461,7 +8511,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <f t="shared" si="1"/>
         <v>3.1249999999999989E-3</v>
@@ -8482,7 +8532,7 @@
         <v>0.28399999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <f>TIME(0,0,15)+A20</f>
         <v>3.2986111111111098E-3</v>
@@ -8503,7 +8553,7 @@
         <v>0.29499999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <f>TIME(0,0,15)+A21</f>
         <v>3.4722222222222207E-3</v>
@@ -8534,28 +8584,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+      <selection activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -8566,16 +8616,16 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1.7361111111111112E-4</v>
       </c>
@@ -8595,7 +8645,7 @@
         <v>26.4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A9" si="0">TIME(0,0,15)+A3</f>
         <v>3.4722222222222224E-4</v>
@@ -8616,7 +8666,7 @@
         <v>95.867000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>5.2083333333333333E-4</v>
@@ -8637,7 +8687,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>6.9444444444444447E-4</v>
@@ -8658,7 +8708,7 @@
         <v>227.667</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>8.6805555555555562E-4</v>
@@ -8679,7 +8729,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>1.0416666666666667E-3</v>
@@ -8700,7 +8750,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>1.2152777777777778E-3</v>
@@ -8721,7 +8771,7 @@
         <v>409.33300000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f t="shared" ref="A10:A20" si="1">TIME(0,0,15)+A9</f>
         <v>1.3888888888888889E-3</v>
@@ -8742,7 +8792,7 @@
         <v>468.06700000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <f t="shared" si="1"/>
         <v>1.5625000000000001E-3</v>
@@ -8763,7 +8813,7 @@
         <v>524.53300000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <f t="shared" si="1"/>
         <v>1.7361111111111112E-3</v>
@@ -8784,7 +8834,7 @@
         <v>572.20000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f t="shared" si="1"/>
         <v>1.9097222222222224E-3</v>
@@ -8805,7 +8855,7 @@
         <v>561.79999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <f t="shared" si="1"/>
         <v>2.0833333333333333E-3</v>
@@ -8826,7 +8876,7 @@
         <v>625.93299999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <f t="shared" si="1"/>
         <v>2.2569444444444442E-3</v>
@@ -8847,7 +8897,7 @@
         <v>679.26700000000005</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <f t="shared" si="1"/>
         <v>2.4305555555555552E-3</v>
@@ -8868,7 +8918,7 @@
         <v>758.66700000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <f t="shared" si="1"/>
         <v>2.6041666666666661E-3</v>
@@ -8889,7 +8939,7 @@
         <v>818.6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <f t="shared" si="1"/>
         <v>2.777777777777777E-3</v>
@@ -8910,7 +8960,7 @@
         <v>868.46699999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <f t="shared" si="1"/>
         <v>2.9513888888888879E-3</v>
@@ -8931,7 +8981,7 @@
         <v>858.2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <f t="shared" si="1"/>
         <v>3.1249999999999989E-3</v>
@@ -8952,7 +9002,7 @@
         <v>816.33299999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <f>TIME(0,0,15)+A20</f>
         <v>3.2986111111111098E-3</v>
@@ -8973,7 +9023,7 @@
         <v>838.86699999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <f>TIME(0,0,15)+A21</f>
         <v>3.4722222222222207E-3</v>

</xml_diff>